<commit_message>
check point with shawn
</commit_message>
<xml_diff>
--- a/db_script/allHeaders.xlsx
+++ b/db_script/allHeaders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repo\Remittance-Web-Portal\db_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DB3E7B-058E-4BCA-AFC4-4D588015AFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F736182-B08D-48F1-8138-11769A2E141D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
   <si>
     <t>EverywhereRemit</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>sAccountNumber</t>
+  </si>
+  <si>
+    <t>TransferAmount</t>
   </si>
 </sst>
 </file>
@@ -1194,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1362,6 +1365,9 @@
       <c r="V2" t="s">
         <v>54</v>
       </c>
+      <c r="W2" t="s">
+        <v>108</v>
+      </c>
       <c r="X2" t="s">
         <v>55</v>
       </c>
@@ -1531,7 +1537,7 @@
       <c r="V4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="2" t="s">
         <v>95</v>
       </c>
       <c r="X4" s="2" t="s">

</xml_diff>